<commit_message>
updated BillTransferAndRetrieve Sheet 5 added SEC
</commit_message>
<xml_diff>
--- a/BillTransferAndRetrieve.xlsx
+++ b/BillTransferAndRetrieve.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SoapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E12FE7D-2A7E-4B97-9AE7-961A8A704B44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D70A80-D063-4FAD-AC5C-902EF70E11A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="4" xr2:uid="{4F2A79EC-6A37-424B-B8E0-534D8D74EB57}"/>
+    <workbookView xWindow="-17880" yWindow="1950" windowWidth="17010" windowHeight="13935" activeTab="4" xr2:uid="{4F2A79EC-6A37-424B-B8E0-534D8D74EB57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="165">
   <si>
     <t>Notes</t>
   </si>
@@ -523,6 +523,15 @@
   </si>
   <si>
     <t>Crofton</t>
+  </si>
+  <si>
+    <t>SEC</t>
+  </si>
+  <si>
+    <t>TEL</t>
+  </si>
+  <si>
+    <t>CCD</t>
   </si>
 </sst>
 </file>
@@ -1141,6 +1150,9 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1926,6 +1938,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2059,6 +2074,9 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2351,16 +2369,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4205A886-25EE-4B75-BC6C-4644EF1A3C3B}">
-  <dimension ref="A1:AE10"/>
+  <dimension ref="A1:AF10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A4" sqref="A4:XFD4"/>
+      <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AF8" sqref="AF8:AF10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2391,7 +2412,7 @@
     <col min="32" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2485,8 +2506,11 @@
       <c r="AE1" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF1" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>119</v>
       </c>
@@ -2574,8 +2598,11 @@
       <c r="AE2" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF2" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>120</v>
       </c>
@@ -2630,8 +2657,11 @@
       <c r="AE3" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF3" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>121</v>
       </c>
@@ -2689,8 +2719,11 @@
       <c r="AE4" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF4" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>122</v>
       </c>
@@ -2778,8 +2811,11 @@
       <c r="AE5" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF5" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>123</v>
       </c>
@@ -2834,8 +2870,11 @@
       <c r="AE6" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF6" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>124</v>
       </c>
@@ -2893,8 +2932,11 @@
       <c r="AE7" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF7" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>125</v>
       </c>
@@ -2982,8 +3024,11 @@
       <c r="AE8" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF8" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>126</v>
       </c>
@@ -3038,8 +3083,11 @@
       <c r="AE9" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF9" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>127</v>
       </c>
@@ -3097,8 +3145,14 @@
       <c r="AE10" s="1" t="s">
         <v>137</v>
       </c>
+      <c r="AF10" s="1" t="s">
+        <v>164</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>